<commit_message>
updated power consumption docs
</commit_message>
<xml_diff>
--- a/calc_power_consumption.xlsx
+++ b/calc_power_consumption.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Configuration values:</t>
   </si>
@@ -130,15 +130,6 @@
   </si>
   <si>
     <t>CR2023, 200 mAh</t>
-  </si>
-  <si>
-    <t>bei avg. 13 mAs läuft der Timer (m):</t>
-  </si>
-  <si>
-    <t>200 mAh =  12000 mAmin</t>
-  </si>
-  <si>
-    <t>oder in h:</t>
   </si>
   <si>
     <t>5 leds, 12 sec/step, one cycle one minute</t>
@@ -214,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -249,21 +240,14 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="29">
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -461,6 +445,16 @@
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -509,39 +503,39 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle3" displayName="Tabelle3" ref="A12:C17" totalsRowCount="1" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A12:C16"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Spalte1" totalsRowLabel="Ergebnis" dataDxfId="22" totalsRowDxfId="2"/>
-    <tableColumn id="2" name="Comment" dataDxfId="21" totalsRowDxfId="1"/>
-    <tableColumn id="3" name="avg. Consumption mAs" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Spalte1" totalsRowLabel="Ergebnis" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="2" name="Comment" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="3" name="avg. Consumption mAs" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="F16:L24" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="F16:L24" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="F16:L24"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="start time, 12s interval" dataDxfId="17"/>
-    <tableColumn id="2" name="Spalte1" dataDxfId="16"/>
-    <tableColumn id="3" name="Spalte2" dataDxfId="15"/>
-    <tableColumn id="4" name="duration sec" dataDxfId="14"/>
-    <tableColumn id="5" name="Spalte3" dataDxfId="13"/>
-    <tableColumn id="6" name="Spalte4" dataDxfId="12"/>
-    <tableColumn id="7" name="Spalte5" dataDxfId="11"/>
+    <tableColumn id="1" name="start time, 12s interval" dataDxfId="14"/>
+    <tableColumn id="2" name="Spalte1" dataDxfId="13"/>
+    <tableColumn id="3" name="Spalte2" dataDxfId="12"/>
+    <tableColumn id="4" name="duration sec" dataDxfId="11"/>
+    <tableColumn id="5" name="Spalte3" dataDxfId="10"/>
+    <tableColumn id="6" name="Spalte4" dataDxfId="9"/>
+    <tableColumn id="7" name="Spalte5" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabelle5" displayName="Tabelle5" ref="G2:K14" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabelle5" displayName="Tabelle5" ref="G2:K14" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="G2:K14"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Step = #led on" dataDxfId="7"/>
-    <tableColumn id="2" name="mA" dataDxfId="6"/>
-    <tableColumn id="3" name="Diff" dataDxfId="5"/>
-    <tableColumn id="4" name="avg" dataDxfId="4"/>
-    <tableColumn id="5" name="Spalte1" dataDxfId="3"/>
+    <tableColumn id="1" name="Step = #led on" dataDxfId="4"/>
+    <tableColumn id="2" name="mA" dataDxfId="3"/>
+    <tableColumn id="3" name="Diff" dataDxfId="2"/>
+    <tableColumn id="4" name="avg" dataDxfId="1"/>
+    <tableColumn id="5" name="Spalte1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -837,7 +831,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,11 +1118,11 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C15" s="7">
         <f>K24</f>
-        <v>11.721599999999997</v>
+        <v>8.139999999999997</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1167,7 +1161,7 @@
       </c>
       <c r="C17" s="7">
         <f>SUBTOTAL(109,Tabelle3[avg. Consumption mAs])</f>
-        <v>12.988999999999997</v>
+        <v>9.4073999999999973</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>18</v>
@@ -1193,7 +1187,10 @@
         <f t="shared" ref="J18:J23" si="1">I18*$B$7 *(1/2+H18)</f>
         <v>19.535999999999994</v>
       </c>
-      <c r="K18" s="7"/>
+      <c r="K18" s="7">
+        <f>Tabelle4[[#This Row],[Spalte3]]/12</f>
+        <v>1.6279999999999994</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F19" s="1">
@@ -1212,18 +1209,19 @@
         <f t="shared" si="1"/>
         <v>58.607999999999983</v>
       </c>
-      <c r="K19" s="7"/>
+      <c r="K19" s="7">
+        <f>Tabelle4[[#This Row],[Spalte3]]/12</f>
+        <v>4.8839999999999986</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="7">
-        <f>12000/13</f>
-        <v>923.07692307692309</v>
+      <c r="B20" s="12"/>
+      <c r="C20" s="11">
+        <f>200/9.41</f>
+        <v>21.253985122210413</v>
       </c>
       <c r="F20" s="1">
         <v>24</v>
@@ -1241,16 +1239,12 @@
         <f t="shared" si="1"/>
         <v>97.679999999999978</v>
       </c>
-      <c r="K20" s="7"/>
+      <c r="K20" s="7">
+        <f>Tabelle4[[#This Row],[Spalte3]]/12</f>
+        <v>8.1399999999999988</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="11">
-        <f>C20/60</f>
-        <v>15.384615384615385</v>
-      </c>
       <c r="F21" s="1">
         <v>36</v>
       </c>
@@ -1267,12 +1261,12 @@
         <f t="shared" si="1"/>
         <v>136.75199999999995</v>
       </c>
-      <c r="K21" s="7"/>
+      <c r="K21" s="7">
+        <f>Tabelle4[[#This Row],[Spalte3]]/12</f>
+        <v>11.395999999999995</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="F22" s="1">
         <v>48</v>
       </c>
@@ -1289,35 +1283,26 @@
         <f t="shared" si="1"/>
         <v>175.82399999999996</v>
       </c>
-      <c r="K22" s="7"/>
+      <c r="K22" s="7">
+        <f>Tabelle4[[#This Row],[Spalte3]]/12</f>
+        <v>14.651999999999996</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F23" s="1">
         <v>60</v>
       </c>
-      <c r="G23" s="1">
-        <v>1</v>
-      </c>
-      <c r="H23" s="1">
-        <v>5</v>
-      </c>
-      <c r="I23" s="1">
-        <v>12</v>
-      </c>
-      <c r="J23" s="7">
-        <f t="shared" si="1"/>
-        <v>214.89599999999993</v>
-      </c>
+      <c r="J23" s="7"/>
       <c r="K23" s="7"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J24" s="11">
         <f>SUM(J18:J23)</f>
-        <v>703.29599999999982</v>
+        <v>488.39999999999986</v>
       </c>
       <c r="K24" s="11">
         <f>J24/60</f>
-        <v>11.721599999999997</v>
+        <v>8.139999999999997</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>21</v>

</xml_diff>